<commit_message>
update files and script
</commit_message>
<xml_diff>
--- a/silva_nochloronomito_taxa_table_ps20.xlsx
+++ b/silva_nochloronomito_taxa_table_ps20.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliemeyer/Documents/GitHub/McH1-7_field_trials_BS2andBS3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliemeyer/Documents/GitHub/McH1-7_field_trials_BS2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8517C8DC-81FD-B042-82BD-CD21599230EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8621AF02-F0AC-D547-8471-84AB66D19C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="19380" windowHeight="13280" xr2:uid="{67051B71-31E4-CB46-9F52-E7DBB2CBE388}"/>
+    <workbookView xWindow="740" yWindow="500" windowWidth="19380" windowHeight="13280" xr2:uid="{67051B71-31E4-CB46-9F52-E7DBB2CBE388}"/>
   </bookViews>
   <sheets>
     <sheet name="silva_nochloronomito_taxa_table" sheetId="1" r:id="rId1"/>
@@ -1161,12 +1161,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{062B9CE0-EB2D-8640-ACFB-18CC3DF47594}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H21"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="4" max="4" width="27.1640625" customWidth="1"/>
     <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1196,59 +1197,59 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>59</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="H2" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="H3" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -1257,24 +1258,24 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="H4" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -1283,24 +1284,24 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="H5" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -1309,24 +1310,24 @@
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="F6" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G6" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="H6" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -1341,18 +1342,18 @@
         <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="G7" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H7" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -1361,50 +1362,50 @@
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G8" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="H8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="G9" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="H9" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -1422,15 +1423,15 @@
         <v>11</v>
       </c>
       <c r="G10" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>70</v>
+        <v>45</v>
+      </c>
+      <c r="H10" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
@@ -1439,24 +1440,24 @@
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="G11" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="H11" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
@@ -1468,21 +1469,21 @@
         <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="G12" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="H12" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
@@ -1491,24 +1492,24 @@
         <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="E13" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="G13" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="H13" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
@@ -1526,15 +1527,15 @@
         <v>11</v>
       </c>
       <c r="G14" t="s">
-        <v>45</v>
-      </c>
-      <c r="H14" t="s">
-        <v>81</v>
+        <v>12</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
@@ -1546,16 +1547,16 @@
         <v>9</v>
       </c>
       <c r="E15" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F15" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="G15" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="H15" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -1586,33 +1587,33 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="E17" t="s">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="F17" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="G17" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="H17" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
@@ -1633,12 +1634,12 @@
         <v>16</v>
       </c>
       <c r="H18" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
@@ -1653,68 +1654,77 @@
         <v>14</v>
       </c>
       <c r="F19" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="G19" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="H19" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="D20" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="E20" t="s">
-        <v>59</v>
+        <v>14</v>
       </c>
       <c r="F20" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="G20" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="H20" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="B21" t="s">
         <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="D21" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="E21" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="F21" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="G21" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="H21" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H21">
+    <sortCondition ref="B2:B21"/>
+    <sortCondition ref="C2:C21"/>
+    <sortCondition ref="D2:D21"/>
+    <sortCondition ref="E2:E21"/>
+    <sortCondition ref="F2:F21"/>
+    <sortCondition ref="G2:G21"/>
+    <sortCondition ref="H2:H21"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>